<commit_message>
arrumando os nomes dos pagotes
</commit_message>
<xml_diff>
--- a/target/bancoDados.xlsx
+++ b/target/bancoDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.silva\Desktop\projeto\hub_bdd\target\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A610FA8-57F6-4D9F-92CD-678E72129502}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC2308E-25F3-4760-92F8-1C55913DF72A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
   </bookViews>
@@ -138,7 +138,7 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>saulosjss63</t>
+    <t>saulosjss64</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
coloquei a class page object manager
</commit_message>
<xml_diff>
--- a/target/bancoDados.xlsx
+++ b/target/bancoDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.silva\Desktop\projeto\hub_bdd\target\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC2308E-25F3-4760-92F8-1C55913DF72A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20721DCF-FF57-4AE9-9CAF-F2539C21CEEA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
   </bookViews>
@@ -138,7 +138,7 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>saulosjss64</t>
+    <t>saulosjss70</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
coloquei web driver manager, page object manager e esta tirando print da tela
</commit_message>
<xml_diff>
--- a/target/bancoDados.xlsx
+++ b/target/bancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.silva\Desktop\projeto\hub_bdd\target\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20721DCF-FF57-4AE9-9CAF-F2539C21CEEA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE2F70F-D587-4BC0-8A80-BBA848050825}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
+    <workbookView xWindow="28680" yWindow="3525" windowWidth="15600" windowHeight="11160" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>saulo.silva@rsinet.com.br</t>
   </si>
   <si>
-    <t>suaMae12</t>
-  </si>
-  <si>
     <t>Saulo</t>
   </si>
   <si>
@@ -138,7 +135,10 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>saulosjss70</t>
+    <t>manodoCeu12</t>
+  </si>
+  <si>
+    <t>saulosjs80</t>
   </si>
 </sst>
 </file>
@@ -510,9 +510,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="22.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -559,7 +559,7 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -570,75 +570,75 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
       <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
         <v>33</v>
-      </c>
-      <c r="M2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
       <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
         <v>30</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>32</v>
-      </c>
-      <c r="L3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>